<commit_message>
Added Svelte cheatsheet, and edited Java
</commit_message>
<xml_diff>
--- a/Java Cheatsheat.xlsx
+++ b/Java Cheatsheat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\OneDrive - University of Kent\COMP3200 - Object Oriented Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D5067-56AD-4E3D-877C-8420ADA8C736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC524E07-E19C-4A65-B11B-DB16A181B9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="711" firstSheet="9" activeTab="10" xr2:uid="{56C432A1-B685-497B-B7E7-0CC1A02FC8F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="711" firstSheet="2" activeTab="9" xr2:uid="{56C432A1-B685-497B-B7E7-0CC1A02FC8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Stuff" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="262">
   <si>
     <t>Concept</t>
   </si>
@@ -1230,9 +1230,6 @@
 }</t>
   </si>
   <si>
-    <t>This is one method to throw an exception into Java code. With this example, we see whether a number is below 0, and if it is, it ends the program, and prints an error message.</t>
-  </si>
-  <si>
     <t xml:space="preserve">If we want to save the IllegalArgumentException to be used at a later time, we can assign it to a RuntimeException variable like this:
 if (key == null) {
   RuntimeException ex = new IllegalArgumentException("nah");
@@ -1470,12 +1467,300 @@
 If we include a message after the assert, then this means that if the condition fails, then the program will end, and it will print out this message. Most of the time, it just makes sense to include a statement after the condition.
 Assert is used heavily within Java text classes, and because the condition has to return a boolean, we can have the condition be a function/method that returns a boolean.</t>
   </si>
+  <si>
+    <t>Creating checked and unchecked exception</t>
+  </si>
+  <si>
+    <t>Checked exception class:
+public class CustomCheckedException extends Exception {
+    public CustomCheckedException(String message) {
+        ...
+    }
+}
+Unchecked exception class:
+public class CustomUncheckedException extends RuntimeException {
+    public CustomUncheckedException(String message) {
+        super(message);
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t>When we're using a checked exception within a method, we have to add this to the method:
+public class Example {
+    public void methodThrowingCheckedException</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>() throws CustomCheckedException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {
+        throw new CustomCheckedException("Checked exception occurred");
+}
+When we're using an unchecked exception within a method, we don't need to add this additional text:
+public static void methodThrowingUncheckedException() {
+    throw new CustomUncheckedException("Unchecked exception occurred");
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The simplest way to think about the difference between checked and unchecked exceptions is like this: checked exceptions will end up throwing an error when something is literally impossible to do (e.g. trying to read a file that isn't there), whereas unchecked exceptions will throw an error when you get an unexpected bug or mistake in the program (e.g. with week 8 homework, having a departure date before an arrival date isn't illegal/impossible, but we're ending the program early because otherwise our code won't work. For the example, by adding an unchecked exception into the constructor as the booking is taking place (as the Booking object is being created), we are forcing the program to end before it constructs arrival and departure dates that are impossible.
+ChatGPT says:
+Checked exceptions are like teachers who insist you complete your homework before leaving class. They force you to acknowledge potential problems (exceptions) and handle them responsibly. You must either catch them (handle the problem) or declare that your method might throw them to someone else.
+Unchecked exceptions are like your friend who suddenly trips over a rock while walking. They represent unexpected issues, like bugs or mistakes in your program's logic. You're not forced to handle them explicitly; they're more of a surprise, like unexpected behavior.
+We define a checked exception class by using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extends Exception</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and we defined an unchecked exception class by using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>extends RuntimeException.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+It's kind of complicated to remember, especially since they're pretty similar, but these are the ways that you do it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Passing checked exceptions between a so-called </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">parent </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">method and a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">child </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>method (another method that is called within the upper method)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example parent method:
+public Booking bookARoom(String roomID, Date arrivalDate, Date departureDate) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>throws BookingFailureException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {
+        Room theRoom = listOfRooms.get(roomID);
+        theRoom.book(arrivalDate, departureDate);,,,
+    }
+Child method:
+public void book(Date arrival, Date departure) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>throws BookingFailureException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    {
+        if(isAvailable(arrival, departure)) {
+            ... Do the booking as normal        
+        } else {
+            throw new BookingFailureException(id, arrival, departure);
+        }
+    }</t>
+    </r>
+  </si>
+  <si>
+    <t>When we have a parent method that calls a child method, and the child method has a checked exception within it, we need to add a throws CheckedExceptionName to the child method, as well as the parent method. This is because, in a sense, the parent method is reponsible for running the child method, and when we introduce a Checked exception to the child, the parent has to take on this responsibility also, which requires it to have a throws CheckedExceptionName in the method header.
+This is a slightly difficult concept to explain, so I'll let ChatGPT provide an example:
+In simple terms, bookARoom is like the team leader overseeing the booking process. When it asks the book method to handle the booking part, it also takes responsibility for any issues that might arise during that process.
+So, when book encounters a problem (like the room being unavailable), it throws a BookingFailureException to signal that something went wrong. And since bookARoom is overseeing the whole process, it's ready to catch and handle this exception if it occurs.
+This ensures that the booking process runs smoothly, even if there are bumps along the way. It's all about making sure everything is taken care of properly!
+Note that you only have to do this (add this syntax to the parent and child methods) if you have a checked exception. If the book method has an unchecked exception, you wouldn't need to worry about this.</t>
+  </si>
+  <si>
+    <t>Printing the stack trace</t>
+  </si>
+  <si>
+    <r>
+      <t>try {
+  book.save(filename);
+  saved = true;
+catch(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Exception </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e) {
+  e.printStrackTrace();
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>If you want to print out the error message directly, you can use catch (Exception e), and then use printStackTrace() to print out the error message normally.</t>
+  </si>
+  <si>
+    <r>
+      <t>This is one method to throw an exception into Java code. With this example, we see whether a number is below 0, and if it is, it ends the program, and prints an error message.
+NOTE: if you don’t know what kind of error you're going to get, or you just want to catch all the different ypes of errors, you can just use Exception e within a catch statement:
+try {
+...
+}
+catch (e</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xception e) {
+...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1643,7 +1928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1692,9 +1977,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1702,6 +1984,32 @@
   <dxfs count="94">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1736,32 +2044,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -3535,13 +3817,13 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}" name="Table11" displayName="Table11" ref="A1:D8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A1:D8" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}" name="Table11" displayName="Table11" ref="A1:D11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+  <autoFilter ref="A1:D11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{23D9BD2F-7AF0-4473-A452-8579FF60CB21}" name="Concept" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{03863FA7-E2E7-45B2-AA55-9A0494115495}" name="Example Code" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8C8FA720-79D9-4483-BA83-D397D654932B}" name="Explained" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{82F43F47-9153-4151-9859-CDA975621954}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{23D9BD2F-7AF0-4473-A452-8579FF60CB21}" name="Concept" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{03863FA7-E2E7-45B2-AA55-9A0494115495}" name="Example Code" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{8C8FA720-79D9-4483-BA83-D397D654932B}" name="Explained" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{82F43F47-9153-4151-9859-CDA975621954}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3626,8 +3908,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}" name="Table8" displayName="Table8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="A1:D8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}" name="Table8" displayName="Table8" ref="A1:D7" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="A1:D7" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0C31EF2F-441F-4E55-B1C8-1555F94F8046}" name="Concept" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{91FBA7EB-A177-4E14-85E5-7D2821C5A180}" name="Example Code" dataDxfId="27"/>
@@ -3950,11 +4232,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BE3793-8F53-49A5-813B-F427F01B1B9E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.140625" style="1" bestFit="1" customWidth="1"/>
@@ -3963,7 +4245,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3977,7 +4259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3987,7 +4269,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="90">
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -4001,7 +4283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120">
+    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -4013,7 +4295,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="90">
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4027,7 +4309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90">
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4039,7 +4321,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="105">
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -4051,7 +4333,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -4063,7 +4345,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="135">
+    <row r="9" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -4075,7 +4357,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
@@ -4087,7 +4369,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="150">
+    <row r="11" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -4101,7 +4383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -4113,7 +4395,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="90">
+    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
@@ -4127,7 +4409,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -4139,7 +4421,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" ht="135">
+    <row r="15" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
@@ -4153,7 +4435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="135">
+    <row r="16" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>54</v>
       </c>
@@ -4167,7 +4449,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="165">
+    <row r="17" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
@@ -4181,7 +4463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="105">
+    <row r="18" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
@@ -4195,7 +4477,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -4213,11 +4495,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E6CB52-2A79-48E7-8C34-52C685FFA217}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="1" customWidth="1"/>
@@ -4226,7 +4508,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4240,7 +4522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="195">
+    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>185</v>
       </c>
@@ -4252,7 +4534,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="120">
+    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>191</v>
       </c>
@@ -4264,7 +4546,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="405">
+    <row r="4" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>194</v>
       </c>
@@ -4278,7 +4560,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="165">
+    <row r="5" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>198</v>
       </c>
@@ -4292,7 +4574,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="165">
+    <row r="6" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>202</v>
       </c>
@@ -4306,7 +4588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90">
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>206</v>
       </c>
@@ -4318,7 +4600,7 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="150">
+    <row r="8" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>226</v>
       </c>
@@ -4340,22 +4622,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E80B6F-1D3E-43E2-9CCC-0B6397F12E90}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="91.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="115.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="168" style="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4369,7 +4651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="195">
+    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>232</v>
       </c>
@@ -4377,79 +4659,116 @@
         <v>233</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="60">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="120">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="105">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="195">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="195">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="B8" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="165">
-      <c r="A8" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>249</v>
+      <c r="B9" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4459,10 +4778,10 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="51.140625" style="1" bestFit="1" customWidth="1"/>
@@ -4471,7 +4790,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4485,7 +4804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="195">
+    <row r="2" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>49</v>
       </c>
@@ -4499,7 +4818,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>65</v>
       </c>
@@ -4513,7 +4832,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
@@ -4525,7 +4844,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>75</v>
       </c>
@@ -4537,7 +4856,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>78</v>
       </c>
@@ -4549,7 +4868,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="60">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>71</v>
       </c>
@@ -4563,7 +4882,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60">
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>123</v>
       </c>
@@ -4575,7 +4894,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>126</v>
       </c>
@@ -4599,11 +4918,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9075256-A2B1-4755-9D84-5845893E10FD}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4612,7 +4931,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4626,7 +4945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75">
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>107</v>
       </c>
@@ -4640,7 +4959,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -4652,7 +4971,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="105">
+    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>112</v>
       </c>
@@ -4666,7 +4985,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>115</v>
       </c>
@@ -4680,7 +4999,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135">
+    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>165</v>
       </c>
@@ -4694,7 +5013,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="120">
+    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>181</v>
       </c>
@@ -4724,7 +5043,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.140625" style="1" bestFit="1" customWidth="1"/>
@@ -4733,7 +5052,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +5066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>105</v>
       </c>
@@ -4757,7 +5076,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>82</v>
       </c>
@@ -4767,7 +5086,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>86</v>
       </c>
@@ -4777,7 +5096,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>88</v>
       </c>
@@ -4791,7 +5110,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>128</v>
       </c>
@@ -4803,7 +5122,7 @@
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>162</v>
       </c>
@@ -4825,11 +5144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8EB8C1-E18B-417A-9A38-E18A2EB61A2E}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -4837,7 +5156,7 @@
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4851,7 +5170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75">
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
@@ -4863,7 +5182,7 @@
       </c>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:4" ht="135">
+    <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
@@ -4875,7 +5194,7 @@
       </c>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:4" ht="60">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>120</v>
       </c>
@@ -4887,7 +5206,7 @@
       </c>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:4" ht="135">
+    <row r="5" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>209</v>
       </c>
@@ -4901,7 +5220,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="135">
+    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>217</v>
       </c>
@@ -4913,7 +5232,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>219</v>
       </c>
@@ -4925,7 +5244,7 @@
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="240">
+    <row r="8" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>222</v>
       </c>
@@ -4949,11 +5268,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64704B0A-EE69-4C2D-84B2-96C4E124AEFB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="1" customWidth="1"/>
@@ -4962,7 +5281,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +5295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>91</v>
       </c>
@@ -4990,7 +5309,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -5002,7 +5321,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="75">
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -5014,7 +5333,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="180">
+    <row r="5" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>187</v>
       </c>
@@ -5042,7 +5361,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" customWidth="1"/>
@@ -5050,7 +5369,7 @@
     <col min="4" max="4" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5064,7 +5383,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>132</v>
       </c>
@@ -5076,7 +5395,7 @@
       </c>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:4" ht="75">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>135</v>
       </c>
@@ -5088,7 +5407,7 @@
       </c>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:4" ht="60">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>139</v>
       </c>
@@ -5100,7 +5419,7 @@
       </c>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>153</v>
       </c>
@@ -5112,7 +5431,7 @@
       </c>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>168</v>
       </c>
@@ -5124,7 +5443,7 @@
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="150">
+    <row r="7" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>211</v>
       </c>
@@ -5138,7 +5457,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="165">
+    <row r="8" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>229</v>
       </c>
@@ -5162,11 +5481,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9DA256F-0657-4E15-8701-03E81A1A2068}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="1" customWidth="1"/>
@@ -5175,7 +5494,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5189,7 +5508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>141</v>
       </c>
@@ -5199,7 +5518,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>142</v>
       </c>
@@ -5211,7 +5530,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>147</v>
       </c>
@@ -5223,7 +5542,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>150</v>
       </c>
@@ -5235,7 +5554,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>156</v>
       </c>
@@ -5247,7 +5566,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="135">
+    <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>161</v>
       </c>
@@ -5275,7 +5594,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="67.5703125" style="1" customWidth="1"/>
@@ -5284,7 +5603,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5298,7 +5617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
@@ -5310,7 +5629,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>175</v>
       </c>
@@ -5320,7 +5639,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>177</v>
       </c>

</xml_diff>

<commit_message>
Added Junit and lambda functions
</commit_message>
<xml_diff>
--- a/Java Cheatsheat.xlsx
+++ b/Java Cheatsheat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BF6E50-F2C0-4A0B-AF49-99ED1BD745BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B33273-089C-4834-9C09-4D3227AEF675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-765" windowWidth="14610" windowHeight="15585" tabRatio="711" firstSheet="3" activeTab="4" xr2:uid="{56C432A1-B685-497B-B7E7-0CC1A02FC8F0}"/>
+    <workbookView xWindow="-28920" yWindow="-5835" windowWidth="29040" windowHeight="15720" tabRatio="711" firstSheet="7" activeTab="14" xr2:uid="{56C432A1-B685-497B-B7E7-0CC1A02FC8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Stuff" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="Inheritance and Interface" sheetId="11" r:id="rId10"/>
     <sheet name="Error Handling" sheetId="12" r:id="rId11"/>
     <sheet name="2D and Multi-Dimensional Arrays" sheetId="13" r:id="rId12"/>
-    <sheet name="Recursion" sheetId="14" r:id="rId13"/>
+    <sheet name="Stream" sheetId="15" r:id="rId13"/>
+    <sheet name="JTests" sheetId="16" r:id="rId14"/>
+    <sheet name="Other things" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="350">
   <si>
     <t>Concept</t>
   </si>
@@ -1953,12 +1955,1135 @@
     }
 }</t>
   </si>
+  <si>
+    <t>Basic stream</t>
+  </si>
+  <si>
+    <t>List&lt;Integer&gt; numbers = Arrays.asList(1, 2, 3, 4, 5);
+// Creating a stream from the list
+// This just creates a stream from the list, no additional operations
+numbers.stream(); // Creating a stream from the list of numbers</t>
+  </si>
+  <si>
+    <t>In this example, we have a list of integers numbers. We create a stream from this list using the stream() method of the List interface. However, we are not performing any additional operations on this stream. The purpose of this example is to show the basic creation of a stream without any further processing.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Method and lambda equivalent:
+public void printSighting(Sighting aSighting) {
+    System.out.println(aSighting.getDetails());
+} 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Sighting aSighting) -&gt; {
+    System.out.println(aSighting.getDetails());
+} </t>
+    </r>
+  </si>
+  <si>
+    <t>Creating a lambdas</t>
+  </si>
+  <si>
+    <t>Recursion:
+This method, sayHello(), demonstrates recursion, where a method calls itself. It prints "Hello" to the console and then calls itself again indefinitely, resulting in an infinite recursion. This would eventually lead to a StackOverflowError.
+Normal loop:
+This method, sayHelloLoopVersion(), demonstrates a normal loop using a while loop. It continuously prints "Hello" to the console in an infinite loop, which will run until manually stopped. Unlike the recursive method, this doesn't rely on method calls to repeat the task, making it less prone to stack overflow.</t>
+  </si>
+  <si>
+    <t>This is a traditional method definition in Java. It takes an instance of the Sighting class as a parameter and prints its details by invoking the getDetails() method on the aSighting object:
+public void printSighting(Sighting aSighting) {
+    System.out.println(aSighting.getDetails());
+}
+This is a lambda expression that does the same thing as the method above. Lambdas in Java are a way to define an anonymous function, which can be treated as data. In this case, the lambda expression takes a Sighting object as input and prints its details using the getDetails() method.
+(Sighting aSighting) -&gt; {
+    System.out.println(aSighting.getDetails());
+}
+Both the method and the lambda expression achieve the same functionality of printing the details of a Sighting object. However, the lambda expression provides a more concise and sometimes more expressive way of defining simple operations, especially when they are passed as arguments to other methods or stored in variables.</t>
+  </si>
+  <si>
+    <t>Processing a collection with a lambda</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Traditional method:
+for (Sighting aSighting : sightingList) {
+  System.out.println(aSighting.getDetails());
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Process a collection with a lambda:
+sightingList.forEach (
+  (Sighting aSighting) -&gt; {
+    System.out.println(aSighting.getDetails());
+  });
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>Traditional Method:
+This method iterates through each Sighting object in the sightingList collection using a for-each loop (for (Sighting aSighting : sightingList)). Within each iteration, it prints the details of the current Sighting object using System.out.println(aSighting.getDetails()).
+Lambda Expression for Collection Processing:
+This approach uses the forEach method available for collections in Java. It takes a lambda expression as an argument, which defines the action to be performed on each element of the collection. In this case, the lambda expression (Sighting aSighting) -&gt; { System.out.println(aSighting.getDetails()); } is used. This lambda expression takes a Sighting object as input and prints its details using System.out.println(aSighting.getDetails()).
+Both methods achieve the same result of printing the details of each Sighting object in the sightingList collection. The lambda expression provides a more concise and often more expressive way of defining such operations, especially when dealing with functional interfaces like Consumer (used by forEach) and when the operation can be easily represented as a single method call.</t>
+  </si>
+  <si>
+    <t>Alternative methods of writing lambda functions:
+Infer type: The type of the object can be left out because it can be inferred from the declaration of 'sightingsList' – the objects in the list are Sighting objects.
+sightingList.forEach(
+  (aSighting) -&gt; {
+    System.out.println(aSighting.getDetails());
+  });
+Single parameter: The parentheses can be left out when there is only one parameter.
+sightingList.forEach(
+  aSighting -&gt; {
+    System.out.println(aSighting.getDetails());
+  });
+Single statement: The curly brackets and terminating semicolon can be left out when there is only a single statement in the body of the lambda.
+sightingList.forEach(
+  aSighting -&gt; 
+    System.out.println(aSighting.getDetails());
+  );</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stream using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.map()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method</t>
+    </r>
+  </si>
+  <si>
+    <t>// Example list of strings
+List&lt;String&gt; words = Arrays.asList("apple", "banana", "cherry", "date");
+// Using map to transform each string to its uppercase form
+List&lt;String&gt; uppercaseWords = words.stream()
+    .map(String::toUpperCase)
+    .collect(Collectors.toList());
+// Printing the transformed list
+System.out.println("Uppercase words: " + uppercaseWords);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The map() method in Java Stream is used to transform each element of the stream using the provided mapping function.
+In this example, map(String::toUpperCase) is used to convert each string to its uppercase form.
+The map() operation does not modify the original stream; instead, it creates a new stream with the transformed elements.
+The Collectors.toList() method is used to collect the elements of the stream into a List.
+Java Stream API provides a functional and declarative approach to processing collections, which can lead to more concise and readable code.
+</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; words = Arrays.asList("apple", "banana", "cherry", "date");
+// Using filter to keep only words starting with "a"
+List&lt;String&gt; filteredWords = words.stream()
+    .filter(word -&gt; word.startsWith("a"))
+    .collect(Collectors.toList());
+// Printing the filtered list
+System.out.println("Words starting with 'a': " + filteredWords);</t>
+  </si>
+  <si>
+    <t>The filter() method in Java Stream is used to select elements from the stream based on a given predicate (condition).
+In this example, filter(word -&gt; word.startsWith("a")) is used to keep only those strings that start with the letter "a".
+The filter() operation does not modify the original stream; instead, it creates a new stream with the filtered elements.
+The Collectors.toList() method is used to collect the filtered elements of the stream into a List.
+Java Stream API provides a functional and declarative approach to processing collections, allowing for more concise and readable code.</t>
+  </si>
+  <si>
+    <t>// Example list of numbers
+List&lt;Integer&gt; numbers = Arrays.asList(1, 2, 3, 4, 5);
+// Using reduce to calculate the sum of all numbers
+int sum = numbers.stream()
+    .reduce(0, (acc, num) -&gt; acc + num);</t>
+  </si>
+  <si>
+    <t>The reduce() method in Java Stream is used to combine elements of the stream into a single result.
+In this example, reduce(0, (acc, num) -&gt; acc + num) is used to calculate the sum of all numbers in the list.
+The first argument of reduce() represents the initial value of the accumulation (0 in this case).
+The second argument is a binary operator (lambda expression (acc, num) -&gt; acc + num) that takes two parameters: the accumulated value (acc) and the current element of the stream (num). It defines how to accumulate the elements.
+The result of the reduction operation is returned as the final value.
+Java Stream API provides a functional and declarative approach to processing collections, allowing for more concise and readable code.</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; fruits = Arrays.asList("apple", "banana", "cherry", "date");
+// Using forEach to print each fruit
+fruits.stream()
+    .forEach(fruit -&gt; System.out.println("Fruit: " + fruit));</t>
+  </si>
+  <si>
+    <t>The forEach() method in Java Stream is used to perform an action on each element of the stream.
+In this example, forEach(fruit -&gt; System.out.println("Fruit: " + fruit)) is used to print each fruit in the list.
+The lambda expression (fruit -&gt; System.out.println("Fruit: " + fruit)) represents the action to be performed on each element of the stream. It takes a single parameter (fruit) and prints it to the console with the prefix "Fruit: ".
+The forEach() operation is a terminal operation, which means it triggers the execution of the stream pipeline.
+Java Stream API provides a functional and declarative approach to processing collections, allowing for more concise and readable code.</t>
+  </si>
+  <si>
+    <t>.sorted()</t>
+  </si>
+  <si>
+    <t>List&lt;Integer&gt; numbers = Arrays.asList(3, 7, 1, 9, 5);
+// Using findFirst to get the first even number in the list
+int firstEven = numbers.stream()
+    .filter(num -&gt; num % 2 == 0)
+    .findFirst();
+// Checking if a first even number is present and printing it
+if (firstEven.isPresent()) {
+    System.out.println("First even number: " + firstEven.get());
+} else {
+    System.out.println("No even numbers found.");
+}</t>
+  </si>
+  <si>
+    <t>We use .min() and .max() to find the minimum and maximum values in the numbers list, respectively.
+We directly assign the result to int variables min and max.
+We use .orElseThrow() as a safeguard to throw an exception if the stream operation somehow results in an empty stream, which should not happen in this specific case where we're certain the list contains elements.</t>
+  </si>
+  <si>
+    <t>// Example list of integers
+List&lt;Integer&gt; numbers = Arrays.asList(3, 7, 1, 9, 5);
+// Finding the minimum and maximum values
+int min = numbers.stream().min(Integer::compareTo);
+int max = numbers.stream().max(Integer::compareTo);
+// Printing the results
+min.ifPresent(minValue -&gt; System.out.println("Minimum value: " + minValue));
+max.ifPresent(maxValue -&gt; System.out.println("Maximum value: " + maxValue));</t>
+  </si>
+  <si>
+    <r>
+      <t>Stream using the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .filter()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stream using the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .reduce() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>method</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stream using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.forEach()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.min() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.max()</t>
+    </r>
+  </si>
+  <si>
+    <t>.findFirst() is a terminal operation that returns a number containing the first element of the stream, if any.
+In this example, we use .filter() before .findFirst() to select only even numbers from the stream.
+Using .findFirst() can be useful when you need to find the first element of a stream that meets certain criteria or simply the first element of the stream.</t>
+  </si>
+  <si>
+    <t>We have a list numberStrings containing string representations of numbers.
+We use .stream() to convert the list into a stream.
+We use .mapToInt() to convert each string element into an integer using Integer::parseInt.
+Integer::parseInt is a method reference to the static method parseInt of the Integer class, which converts a string to an integer.
+After mapping each string to an integer, we use .sum() to calculate the sum of the integers.
+The result is stored in the sum variable, which is then printed to the console.
+This approach demonstrates how .mapToInt() is used to transform elements of a stream from one type (in this case, strings) to another type (integers) and perform operations specific to the new type, such as calculating the sum of the integers. It's a common pattern used in Java streams to convert elements to primitive types for efficient processing.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List&lt;String&gt; numberStrings = Arrays.asList("1", "2", "3", "4", "5");
+// Using mapToInt to convert strings to integers and calculate sum
+int sum = numberStrings.stream()
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    .mapToInt(Integer::parseInt)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    .sum();
+// Printing the sum
+System.out.println("Sum of numbers: " + sum);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The .mapToInt() method here could also be done using the .stream() and .forEach():
+List&lt;String&gt; numberStrings = Arrays.asList("1", "2", "3", "4", "5");
+// Using stream and forEach to convert strings to integers and calculate sum
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int[] sum = {0}; // Using an array to store the sum as an int[] to be effectively final for lambda expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+numberStrings.stream()
+    .forEach(numString -&gt; sum += Integer.parseInt(numString));
+// Printing the sum
+System.out.println("Sum of numbers: " + sum[0]);</t>
+    </r>
+  </si>
+  <si>
+    <t>List&lt;String&gt; fruits = Arrays.asList("Apple", "Banana", "Orange", "Grapes");
+// Collecting elements of stream into a list
+List&lt;String&gt; collectedList = fruits.stream()
+    .filter(fruit -&gt; fruit.startsWith("A"))
+    .collect(Collectors.toList());</t>
+  </si>
+  <si>
+    <t>Are alternative to .collect(), such as this:
+String[] collectedArray = fruits.stream()
+    .filter(fruit -&gt; fruit.startsWith("A"))
+    .toArray(String[]::new);</t>
+  </si>
+  <si>
+    <t>We have an example list of strings fruits.
+We use .stream() to convert the list into a stream.
+We use .filter(fruit -&gt; fruit.startsWith("A")) to filter elements of the stream, selecting only those fruits that start with the letter "A".
+We use .collect(Collectors.toList()) to collect the filtered elements into a List&lt;String&gt;.
+The result is a List&lt;String&gt; containing the filtered fruits starting with "A".
+We print the collected list to the console.
+In this example, .collect() is used to accumulate elements of a stream into a collection. The Collectors.toList() collector is used to collect elements into a List. Depending on the collector used with .collect(), you can collect elements into various types of collections, such as lists, sets, or maps.
+TLDR: Once we've done all our filtering/etc, using .collect makes it very easy for us to add these items.</t>
+  </si>
+  <si>
+    <t>.collect()</t>
+  </si>
+  <si>
+    <t>.mapToInt()</t>
+  </si>
+  <si>
+    <t>.findFirst()</t>
+  </si>
+  <si>
+    <t>Streams are a completely optional feature for Java, and in fact in many cases, you are able to use many of the methods shown here in tandem with one another, without the .stream() method. However there are certain advantages to using .stream(), such as parallelism, pipelining, and interopability. But overall, they are entirely optional.</t>
+  </si>
+  <si>
+    <t>List&lt;String&gt; fruits = Arrays.asList("Orange", "Apple", "Banana", "Grapes");
+// Sorting the list of strings in ascending order
+fruits.stream()
+    .sorted() // Sorting the stream
+    .forEach(System.out::println); // Printing each sorted element</t>
+  </si>
+  <si>
+    <t>We have an example list of strings fruits.
+We use .stream() to convert the list into a stream.
+We use .sorted() to sort the elements of the stream in their natural order (ascending order for strings).
+The sorted elements are then printed to the console using .forEach(System.out::println).</t>
+  </si>
+  <si>
+    <t>Basic structure of a Junit test</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The first thing that we need to do is we need to import Test into our program using this line:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">import org.junit.jupiter.api.Test;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">We also need to import all the Assert methods:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">import static org.junit.jupiter.api.Assertions.*;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When we create the Test method, we have to put </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> above any methods which we are going to be using for testing. This basically makes the method within the class ready to check if the method passes or failed.
+Finally, we include a number of assert methods, which basically do a boolean check.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">import org.junit.jupiter.api.Test;
+import static org.junit.jupiter.api.Assertions.*;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+class PartsInventoryTest {
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    void addPart() {
+        PartsInventory inventory = new PartsInventory();
+        Part part1 = new Part(1, "Type1", "AMD", "AMD fan", 33.99);
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertTrue(inventory.addPart(part1));</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        Part newPart = new Part(1, "Type2", "NVIDIA", "NVIDIA fan", 33.99);
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertFalse(inventory.addPart(newPart));</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        Part newPart2 = new Part(3, "Type1", "NVIDIA", "NVIDIA fan", 33.99);
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertTrue(inventory.addPart(newPart2));</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    }</t>
+    </r>
+  </si>
+  <si>
+    <t>Using @BeforeEach to run the initial methods</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">import org.junit.jupiter.api.Test;
+import static org.junit.jupiter.api.Assertions.*;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">import org.junit.jupiter.api.BeforeEach;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">public class PartsInventoryTest {
+  private PartsInventory inventory;
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@BeforeEach
+  public void setup() {
+    System.out.println("Program running.");
+    inventory = new PartsInventory();
+  }</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@BeforeEach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> annotation for a method means that when the test class is run, any method that has this decorator will automatically run. This can be very useful when we want to initialise the tests before we've even started them.
+In the example to the left, we are initialising the inventory for our program. When the test methods are all run, it runs this method each time. If we didn't do this, then for every test method that is tried, we would need to create a new PartsInventory item. This would increase the chances of us making an error, and, in the long run, depending on the number of test method that we have, it may increase the number of lines of code that we produce overall.</t>
+    </r>
+  </si>
+  <si>
+    <t>AssertTrue() and AssertFalse()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void addPart() {
+    PartsInventory inventory = new PartsInventory();
+    Part part1 = new Part(1, "Type1", "AMD", "AMD fan", 33.99);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    assertTrue(inventory.addPart</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>part1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    Part newPart = new Part(1, "Type2", "NVIDIA", "NVIDIA fan", 33.99);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    assertFalse(inventory.addPart</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>newPart</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All of the Assert functions within Java, as well as other languages, are quite difficult to understand, but I'll try to explain these ones.
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertTrue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertFalse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> methods are used to check whether the values that are within the brackets are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> respectively. Although the example to the left includes methods that return boolean values, assertTrue and assertFalse could also take individual variables which are of the boolean types. E.g.:
+boolean alive = true;
+assertTrue(alive);
+If you have assertTrue, and the item within the brackets is false, then it will stop the program from running, and show an error.</t>
+    </r>
+  </si>
+  <si>
+    <t>AssertEqual() and AssertNotEqual()</t>
+  </si>
+  <si>
+    <t>The assertTrue method can be understood using this Python syntax:
+if (inventory.addPart(part1)): # If true
+    pass
+else: # if False
+    [ERROR]
+The assertFalse method can be understood using this Python syntax:
+if !(inventory.addPart(part1)): # if false
+  pass
+else: # if true
+  [ERROR]
+assertTrue and assertFalse actually take a maximum of two values: The first value is an optional custom message that will appear if the assert fails, and the second value is the item that we're testing.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void addPart() {
+    PartsInventory inventory = new PartsInventory();
+    string name = "Conor";
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertEqual(name, "Conor");</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // Will pass this test
+    int number = 40
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertNotEqual(number, 30);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> // Will pass this test</t>
+    </r>
+  </si>
+  <si>
+    <t>assertEqual and assertNotEqual actually take a maximum of three values: The first value is an optional custom message that will appear if the assert fails, and the second and third values are the items item that we're comparing against one another.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">These assert methods are very similar to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertTrue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>assertFalse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, but instead of checking a boolean, they compare two values to see if they're the same or not. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">assertTrue </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">will cause an error if the two items being compared are not the same, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">assertFalse </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>will cause an error if the two items being compared are the same.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1981,6 +3106,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2126,7 +3257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2178,19 +3309,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="126">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2198,6 +3346,127 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4129,169 +5398,195 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16DD788E-5446-4924-B02E-34C6DD58B623}" name="Table1" displayName="Table1" ref="A1:D18" totalsRowShown="0" headerRowDxfId="109" dataDxfId="107" headerRowBorderDxfId="108" tableBorderDxfId="106" totalsRowBorderDxfId="105">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16DD788E-5446-4924-B02E-34C6DD58B623}" name="Table1" displayName="Table1" ref="A1:D18" totalsRowShown="0" headerRowDxfId="125" dataDxfId="123" headerRowBorderDxfId="124" tableBorderDxfId="122" totalsRowBorderDxfId="121">
   <autoFilter ref="A1:D18" xr:uid="{16DD788E-5446-4924-B02E-34C6DD58B623}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3DCD619F-49FC-4EA1-886C-F41A4950CECE}" name="Concept" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{795BB6F0-DD26-4D97-8603-C6455573EC20}" name="Example Code" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{8EBBFAC7-4272-42E4-B8EE-D666174C5505}" name="Explained" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{6591A265-7ADB-44E2-A953-FF7B8DF04EE0}" name="Notes" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{3DCD619F-49FC-4EA1-886C-F41A4950CECE}" name="Concept" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{795BB6F0-DD26-4D97-8603-C6455573EC20}" name="Example Code" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{8EBBFAC7-4272-42E4-B8EE-D666174C5505}" name="Explained" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{6591A265-7ADB-44E2-A953-FF7B8DF04EE0}" name="Notes" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{99619868-832A-405A-B105-72AB3D8B57BA}" name="Table10" displayName="Table10" ref="A1:D8" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{99619868-832A-405A-B105-72AB3D8B57BA}" name="Table10" displayName="Table10" ref="A1:D8" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44">
   <autoFilter ref="A1:D8" xr:uid="{99619868-832A-405A-B105-72AB3D8B57BA}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{53B46DAA-7980-4B0B-863F-E1F380776F90}" name="Concept" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{29C342DE-9140-4480-9266-066B449A4ADC}" name="Example Code" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{37415ECE-FD88-4DA5-8B62-A96A008ECC05}" name="Explained" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{9EC12DE3-F41C-4211-B2F6-F847CC563540}" name="Notes" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{53B46DAA-7980-4B0B-863F-E1F380776F90}" name="Concept" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{29C342DE-9140-4480-9266-066B449A4ADC}" name="Example Code" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{37415ECE-FD88-4DA5-8B62-A96A008ECC05}" name="Explained" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{9EC12DE3-F41C-4211-B2F6-F847CC563540}" name="Notes" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}" name="Table11" displayName="Table11" ref="A1:D11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}" name="Table11" displayName="Table11" ref="A1:D11" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="A1:D11" xr:uid="{6CA9D030-073E-450A-B938-3B2ADD2BB5A8}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{23D9BD2F-7AF0-4473-A452-8579FF60CB21}" name="Concept" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{03863FA7-E2E7-45B2-AA55-9A0494115495}" name="Example Code" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{8C8FA720-79D9-4483-BA83-D397D654932B}" name="Explained" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{82F43F47-9153-4151-9859-CDA975621954}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{23D9BD2F-7AF0-4473-A452-8579FF60CB21}" name="Concept" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{03863FA7-E2E7-45B2-AA55-9A0494115495}" name="Example Code" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{8C8FA720-79D9-4483-BA83-D397D654932B}" name="Explained" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{82F43F47-9153-4151-9859-CDA975621954}" name="Notes" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{03BA445D-CE25-4ADE-9208-35C15B732FB7}" name="Table12" displayName="Table12" ref="A1:D5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{03BA445D-CE25-4ADE-9208-35C15B732FB7}" name="Table12" displayName="Table12" ref="A1:D5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
   <autoFilter ref="A1:D5" xr:uid="{03BA445D-CE25-4ADE-9208-35C15B732FB7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{081D8FE9-AC31-4FFD-AB90-C69165554F17}" name="Concept" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{EFD6B83F-CCAC-4459-ACC2-424679F70913}" name="Example Code" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2CE25502-50B2-4E7F-8A11-18670947FE44}" name="Explained" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{F4D170CF-A5B8-42BE-8301-E055B08E0717}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{081D8FE9-AC31-4FFD-AB90-C69165554F17}" name="Concept" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{EFD6B83F-CCAC-4459-ACC2-424679F70913}" name="Example Code" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{2CE25502-50B2-4E7F-8A11-18670947FE44}" name="Explained" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{F4D170CF-A5B8-42BE-8301-E055B08E0717}" name="Notes" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{759651A4-9E1A-41CE-A30D-79EBF47D6E06}" name="Table13" displayName="Table13" ref="A1:D2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
-  <autoFilter ref="A1:D2" xr:uid="{759651A4-9E1A-41CE-A30D-79EBF47D6E06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{1AE2A51C-5437-4DD8-B3F0-B78B6789599D}" name="Table14" displayName="Table14" ref="A1:D11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+  <autoFilter ref="A1:D11" xr:uid="{1AE2A51C-5437-4DD8-B3F0-B78B6789599D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3D8356EB-21F5-4FDB-9333-7DC07F9340C0}" name="Concept" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{258990E7-1228-49D7-BB63-5792B0CB06BE}" name="Example Code" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1CF789FF-6AF3-495A-BDF6-0D38AB9F5E33}" name="Explained" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{E6B03992-B70F-4235-94AC-E4D20310A29D}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C1EB91BF-AB8D-4A21-B41B-9127E22851DE}" name="Concept" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{9D18D685-A117-418D-8399-70942EF98868}" name="Example Code" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{F1FE4530-9CCF-4F36-AD90-27F71B47A04F}" name="Explained" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{D352E0FF-D5DA-4FC5-8AFB-74B42AEFDEA6}" name="Notes" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B8871262-C6BF-45CD-85DE-FB8A9F4664D2}" name="Table15" displayName="Table15" ref="A1:D5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="A1:D5" xr:uid="{B8871262-C6BF-45CD-85DE-FB8A9F4664D2}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{69644359-49F0-4BA4-A747-4967EE4816EC}" name="Concept" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D086A373-0564-4FD4-B886-8EB331A1F06E}" name="Example Code" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C560E0F0-DBB7-49B5-9C34-91BFCA7E02E6}" name="Explained" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{45CA0401-57CB-48DA-A415-D0036B6ACB4D}" name="Notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{759651A4-9E1A-41CE-A30D-79EBF47D6E06}" name="Table13" displayName="Table13" ref="A1:D4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="A1:D4" xr:uid="{759651A4-9E1A-41CE-A30D-79EBF47D6E06}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3D8356EB-21F5-4FDB-9333-7DC07F9340C0}" name="Concept" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{258990E7-1228-49D7-BB63-5792B0CB06BE}" name="Example Code" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{1CF789FF-6AF3-495A-BDF6-0D38AB9F5E33}" name="Explained" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E6B03992-B70F-4235-94AC-E4D20310A29D}" name="Notes" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EAA5C14-3C65-4D11-8826-F81720205D11}" name="Table2" displayName="Table2" ref="A1:D9" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99" tableBorderDxfId="97" totalsRowBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EAA5C14-3C65-4D11-8826-F81720205D11}" name="Table2" displayName="Table2" ref="A1:D9" totalsRowShown="0" headerRowDxfId="116" dataDxfId="114" headerRowBorderDxfId="115" tableBorderDxfId="113" totalsRowBorderDxfId="112">
   <autoFilter ref="A1:D9" xr:uid="{4EAA5C14-3C65-4D11-8826-F81720205D11}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0286523B-BEEA-41E1-8C80-9FC84008EEF7}" name="Concept" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{2721253F-381F-425C-9A73-FDB7AB48EA24}" name="Example Code" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{07423FA0-42BC-47E1-8A7D-A1AA79BAC7B1}" name="Explained" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{E99197EF-FAD7-47B7-A3FC-1D07236437A3}" name="Notes" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{0286523B-BEEA-41E1-8C80-9FC84008EEF7}" name="Concept" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{2721253F-381F-425C-9A73-FDB7AB48EA24}" name="Example Code" dataDxfId="110"/>
+    <tableColumn id="3" xr3:uid="{07423FA0-42BC-47E1-8A7D-A1AA79BAC7B1}" name="Explained" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{E99197EF-FAD7-47B7-A3FC-1D07236437A3}" name="Notes" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B0D8A73-09BF-4058-9977-F5B44A31B982}" name="Table6" displayName="Table6" ref="A1:D7" totalsRowShown="0" headerRowDxfId="91" dataDxfId="89" headerRowBorderDxfId="90" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B0D8A73-09BF-4058-9977-F5B44A31B982}" name="Table6" displayName="Table6" ref="A1:D7" totalsRowShown="0" headerRowDxfId="107" dataDxfId="105" headerRowBorderDxfId="106" tableBorderDxfId="104">
   <autoFilter ref="A1:D7" xr:uid="{1B0D8A73-09BF-4058-9977-F5B44A31B982}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6C7F8E5C-753C-489B-9BBB-E6A2D8CCF0D4}" name="Concept" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{C885F9F4-5DA8-47C4-9D91-298C5DB74E47}" name="Example Code" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{689939E8-A0B6-451D-8DEC-588F298F8A9F}" name="Explained" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{2FEEFACE-7848-49F4-B710-82ECB90CBFC3}" name="Notes" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{6C7F8E5C-753C-489B-9BBB-E6A2D8CCF0D4}" name="Concept" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{C885F9F4-5DA8-47C4-9D91-298C5DB74E47}" name="Example Code" dataDxfId="102"/>
+    <tableColumn id="3" xr3:uid="{689939E8-A0B6-451D-8DEC-588F298F8A9F}" name="Explained" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{2FEEFACE-7848-49F4-B710-82ECB90CBFC3}" name="Notes" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{113925D8-E616-426C-B752-05B5209B0941}" name="Table3" displayName="Table3" ref="A1:D12" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{113925D8-E616-426C-B752-05B5209B0941}" name="Table3" displayName="Table3" ref="A1:D12" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
   <autoFilter ref="A1:D12" xr:uid="{113925D8-E616-426C-B752-05B5209B0941}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D279EE39-1140-4EC7-949A-6D14FEB9BE0B}" name="Concept" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{5EE9883E-1E98-49FA-83D0-3A18D65FE5E5}" name="Example Code" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{53FE148A-0C0E-4A85-877C-7978F9E3B2B4}" name="Explained" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{AA80B0A0-CFBA-4100-AA07-E4AB062457F2}" name="Notes" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{D279EE39-1140-4EC7-949A-6D14FEB9BE0B}" name="Concept" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{5EE9883E-1E98-49FA-83D0-3A18D65FE5E5}" name="Example Code" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{53FE148A-0C0E-4A85-877C-7978F9E3B2B4}" name="Explained" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{AA80B0A0-CFBA-4100-AA07-E4AB062457F2}" name="Notes" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{89953CEC-BCDC-4366-828C-BB8B0C322B2C}" name="Table4" displayName="Table4" ref="A1:D10" totalsRowShown="0" headerRowDxfId="74" headerRowBorderDxfId="73" tableBorderDxfId="72" totalsRowBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{89953CEC-BCDC-4366-828C-BB8B0C322B2C}" name="Table4" displayName="Table4" ref="A1:D10" totalsRowShown="0" headerRowDxfId="90" headerRowBorderDxfId="89" tableBorderDxfId="88" totalsRowBorderDxfId="87">
   <autoFilter ref="A1:D10" xr:uid="{89953CEC-BCDC-4366-828C-BB8B0C322B2C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B285AC4A-7328-4994-9EAD-4B62E00CDA3D}" name="Concept" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{14DC1609-648D-4687-AAF5-D62AC7D8A9CB}" name="Example Code" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{3BA78236-E608-406B-B385-854EE2A51DDC}" name="Explained" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{3F8A8E22-4D2A-43A6-96F0-D61DF8FE316A}" name="Notes" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{B285AC4A-7328-4994-9EAD-4B62E00CDA3D}" name="Concept" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{14DC1609-648D-4687-AAF5-D62AC7D8A9CB}" name="Example Code" dataDxfId="85"/>
+    <tableColumn id="3" xr3:uid="{3BA78236-E608-406B-B385-854EE2A51DDC}" name="Explained" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{3F8A8E22-4D2A-43A6-96F0-D61DF8FE316A}" name="Notes" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4918BE04-ECC3-4345-9E37-13655BA34C0F}" name="Table5" displayName="Table5" ref="A1:D5" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4918BE04-ECC3-4345-9E37-13655BA34C0F}" name="Table5" displayName="Table5" ref="A1:D5" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A1:D5" xr:uid="{4918BE04-ECC3-4345-9E37-13655BA34C0F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4479719A-91E1-4799-91B0-A3883BF6E05C}" name="Concept" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{AECC58FA-4532-4DFA-B17E-AB02450E8CD6}" name="Example Code" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{2512F099-266D-4B50-B91E-338F289C7689}" name="Explained" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{B2C00F2B-DDE5-46D1-B229-B7D35C9ED297}" name="Notes" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{4479719A-91E1-4799-91B0-A3883BF6E05C}" name="Concept" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{AECC58FA-4532-4DFA-B17E-AB02450E8CD6}" name="Example Code" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{2512F099-266D-4B50-B91E-338F289C7689}" name="Explained" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{B2C00F2B-DDE5-46D1-B229-B7D35C9ED297}" name="Notes" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F9F44F01-7623-426C-B571-4EEADD579B48}" name="Table7" displayName="Table7" ref="A1:D8" totalsRowShown="0" headerRowDxfId="57" headerRowBorderDxfId="56" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F9F44F01-7623-426C-B571-4EEADD579B48}" name="Table7" displayName="Table7" ref="A1:D8" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
   <autoFilter ref="A1:D8" xr:uid="{F9F44F01-7623-426C-B571-4EEADD579B48}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{77A2298F-E32C-406A-86E5-E7CBED575A58}" name="Concept" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{F4C128A5-05EC-4A0E-98F4-A1025C9B2AB3}" name="Example Code" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{63D7EE67-E818-4581-A541-68AD685959E1}" name="Explained" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{459D438E-87C2-4AF9-B614-2725CE4EFD2B}" name="Notes" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{77A2298F-E32C-406A-86E5-E7CBED575A58}" name="Concept" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{F4C128A5-05EC-4A0E-98F4-A1025C9B2AB3}" name="Example Code" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{63D7EE67-E818-4581-A541-68AD685959E1}" name="Explained" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{459D438E-87C2-4AF9-B614-2725CE4EFD2B}" name="Notes" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}" name="Table8" displayName="Table8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}" name="Table8" displayName="Table8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="A1:D8" xr:uid="{6DBA3E09-00BA-425D-BBAD-71CEB29C5732}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0C31EF2F-441F-4E55-B1C8-1555F94F8046}" name="Concept" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{91FBA7EB-A177-4E14-85E5-7D2821C5A180}" name="Example Code" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{1F3ECDB9-5313-4E01-B103-3210990E5C3C}" name="Explained" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{3CB7AEE4-A108-4C70-8537-FA913B55C38B}" name="Notes" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{0C31EF2F-441F-4E55-B1C8-1555F94F8046}" name="Concept" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{91FBA7EB-A177-4E14-85E5-7D2821C5A180}" name="Example Code" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{1F3ECDB9-5313-4E01-B103-3210990E5C3C}" name="Explained" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{3CB7AEE4-A108-4C70-8537-FA913B55C38B}" name="Notes" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6F55A446-6561-4476-AA76-B8BB7233FE59}" name="Table9" displayName="Table9" ref="A1:D4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6F55A446-6561-4476-AA76-B8BB7233FE59}" name="Table9" displayName="Table9" ref="A1:D4" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A1:D4" xr:uid="{6F55A446-6561-4476-AA76-B8BB7233FE59}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4ACA6CE0-7645-4700-AD38-BCC23A63D42B}" name="Concept" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{5361957D-1A9E-42A6-9C87-1AC3CC467C89}" name="Example Code" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{4423DB43-2B74-4E9D-A1B6-2E885958B5C6}" name="Explained" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{7486DEA3-65A8-4699-A2DD-2F915CB1BD24}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{4ACA6CE0-7645-4700-AD38-BCC23A63D42B}" name="Concept" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{5361957D-1A9E-42A6-9C87-1AC3CC467C89}" name="Example Code" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{4423DB43-2B74-4E9D-A1B6-2E885958B5C6}" name="Explained" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{7486DEA3-65A8-4699-A2DD-2F915CB1BD24}" name="Notes" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4983,7 +6278,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5215,17 +6510,17 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48447352-76C6-4397-BD27-13F0910034F4}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CEBCAB-6B42-426A-A5C4-DD0029547C9B}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="89.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="91.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -5245,12 +6540,288 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2130F67-8655-43B4-BDF7-2819530F624A}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.42578125" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48447352-76C6-4397-BD27-13F0910034F4}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>291</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>292</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -5688,7 +7259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8EB8C1-E18B-417A-9A38-E18A2EB61A2E}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -5813,13 +7384,13 @@
       <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="13"/>
     </row>
   </sheetData>
@@ -6467,20 +8038,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6503,6 +8074,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63B59450-9090-446C-8742-92F433D71E0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE214711-5800-4A75-B0F2-B108FB8A159B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5c6232e5-8f1b-49db-befc-69ee02b309f0"/>
@@ -6517,12 +8096,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63B59450-9090-446C-8742-92F433D71E0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>